<commit_message>
add CU and PC, debug a little
</commit_message>
<xml_diff>
--- a/CPU控制指令.xlsx
+++ b/CPU控制指令.xlsx
@@ -511,17 +511,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A7" sqref="A7"/>
+      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="9" style="1"/>
+    <col min="1" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="12" width="9" style="1"/>
     <col min="13" max="13" width="21.875" style="1" customWidth="1"/>
     <col min="14" max="15" width="25.5" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="16" max="16" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -815,10 +818,10 @@
         <v>1</v>
       </c>
       <c r="Q6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -865,10 +868,10 @@
         <v>1</v>
       </c>
       <c r="Q7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add ROMdata, decoder, top, Extend. not debug yet
</commit_message>
<xml_diff>
--- a/CPU控制指令.xlsx
+++ b/CPU控制指令.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
   <si>
     <t>ALUScrA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,6 +178,10 @@
   </si>
   <si>
     <t>nWR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -513,7 +517,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="topRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -940,17 +944,17 @@
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
         <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1</v>
       </c>
       <c r="K9" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
debug and finish simulation(success and no bug)
</commit_message>
<xml_diff>
--- a/CPU控制指令.xlsx
+++ b/CPU控制指令.xlsx
@@ -517,7 +517,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I18" sqref="I18"/>
+      <selection pane="topRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -901,10 +901,10 @@
         <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>12</v>

</xml_diff>